<commit_message>
Implementacion final de notificacion por correo(Enviado,Observado)
</commit_message>
<xml_diff>
--- a/public/cursoTesis-2022/A2021-TRUJILLO.xlsx
+++ b/public/cursoTesis-2022/A2021-TRUJILLO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\proyect-tesis-conta\public\cursoTesis-2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2A8624B-D393-4F4E-924A-A8185F82D900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E43185-794E-42C3-AB57-CD5C4A5BACD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6360" yWindow="915" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="A2021-TRUJILLO" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="28">
   <si>
     <t>NELSON OCTAVIO RUIZ CERDAN</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t>MAURO CESAR ARMAS AGUILAR</t>
+  </si>
+  <si>
+    <t>null</t>
   </si>
 </sst>
 </file>
@@ -941,10 +944,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F1" sqref="F1:F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -953,7 +956,7 @@
     <col min="4" max="4" width="31.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>2641</v>
       </c>
@@ -969,8 +972,11 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2841</v>
       </c>
@@ -986,8 +992,11 @@
       <c r="E2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3387</v>
       </c>
@@ -1003,8 +1012,11 @@
       <c r="E3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1179</v>
       </c>
@@ -1020,8 +1032,11 @@
       <c r="E4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4113</v>
       </c>
@@ -1037,8 +1052,11 @@
       <c r="E5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2149</v>
       </c>
@@ -1054,8 +1072,11 @@
       <c r="E6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4532</v>
       </c>
@@ -1071,8 +1092,11 @@
       <c r="E7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4609</v>
       </c>
@@ -1088,8 +1112,11 @@
       <c r="E8" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4028</v>
       </c>
@@ -1105,8 +1132,11 @@
       <c r="E9" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>5766</v>
       </c>
@@ -1122,8 +1152,11 @@
       <c r="E10" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>5582</v>
       </c>
@@ -1139,8 +1172,11 @@
       <c r="E11" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>5714</v>
       </c>
@@ -1156,8 +1192,11 @@
       <c r="E12" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>5437</v>
       </c>
@@ -1173,8 +1212,11 @@
       <c r="E13" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>4993</v>
       </c>
@@ -1190,8 +1232,11 @@
       <c r="E14" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>5581</v>
       </c>
@@ -1207,8 +1252,11 @@
       <c r="E15" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>5909</v>
       </c>
@@ -1224,8 +1272,11 @@
       <c r="E16" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>5107</v>
       </c>
@@ -1241,8 +1292,11 @@
       <c r="E17" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>6489</v>
       </c>
@@ -1258,8 +1312,11 @@
       <c r="E18" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>5125</v>
       </c>
@@ -1275,8 +1332,11 @@
       <c r="E19" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>5127</v>
       </c>
@@ -1292,8 +1352,11 @@
       <c r="E20" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>6430</v>
       </c>
@@ -1309,8 +1372,11 @@
       <c r="E21" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>5132</v>
       </c>
@@ -1325,6 +1391,9 @@
       </c>
       <c r="E22" t="s">
         <v>3</v>
+      </c>
+      <c r="F22" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implementacion de MAILs y Orcid para el asesor
</commit_message>
<xml_diff>
--- a/public/cursoTesis-2022/A2021-TRUJILLO.xlsx
+++ b/public/cursoTesis-2022/A2021-TRUJILLO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\proyect-tesis-conta\public\cursoTesis-2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E43185-794E-42C3-AB57-CD5C4A5BACD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02803D57-7931-4089-8046-AC1CEFD1E1A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="50">
   <si>
     <t>NELSON OCTAVIO RUIZ CERDAN</t>
   </si>
@@ -104,13 +104,79 @@
   </si>
   <si>
     <t>null</t>
+  </si>
+  <si>
+    <t>0000-0003-3388-4343</t>
+  </si>
+  <si>
+    <t>0000-0003-3388-4344</t>
+  </si>
+  <si>
+    <t>0000-0003-3388-4345</t>
+  </si>
+  <si>
+    <t>0000-0003-3388-4346</t>
+  </si>
+  <si>
+    <t>0000-0003-3388-4347</t>
+  </si>
+  <si>
+    <t>0000-0003-3388-4348</t>
+  </si>
+  <si>
+    <t>0000-0003-3388-4349</t>
+  </si>
+  <si>
+    <t>0000-0003-3388-4350</t>
+  </si>
+  <si>
+    <t>0000-0003-3388-4351</t>
+  </si>
+  <si>
+    <t>0000-0003-3388-4352</t>
+  </si>
+  <si>
+    <t>0000-0003-3388-4353</t>
+  </si>
+  <si>
+    <t>0000-0003-3388-4354</t>
+  </si>
+  <si>
+    <t>0000-0003-3388-4355</t>
+  </si>
+  <si>
+    <t>0000-0003-3388-4356</t>
+  </si>
+  <si>
+    <t>0000-0003-3388-4357</t>
+  </si>
+  <si>
+    <t>0000-0003-3388-4358</t>
+  </si>
+  <si>
+    <t>0000-0003-3388-4359</t>
+  </si>
+  <si>
+    <t>0000-0003-3388-4360</t>
+  </si>
+  <si>
+    <t>0000-0003-3388-4361</t>
+  </si>
+  <si>
+    <t>0000-0003-3388-4362</t>
+  </si>
+  <si>
+    <t>0000-0003-3388-4363</t>
+  </si>
+  <si>
+    <t>0000-0003-3388-4364</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -241,6 +307,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -944,19 +1016,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F22"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="39.140625" customWidth="1"/>
-    <col min="4" max="4" width="31.140625" customWidth="1"/>
+    <col min="2" max="3" width="39.140625" customWidth="1"/>
+    <col min="5" max="5" width="31.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>2641</v>
       </c>
@@ -964,19 +1036,22 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2841</v>
       </c>
@@ -984,19 +1059,22 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3387</v>
       </c>
@@ -1004,19 +1082,22 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1179</v>
       </c>
@@ -1024,19 +1105,22 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="G4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4113</v>
       </c>
@@ -1044,19 +1128,22 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s">
         <v>8</v>
       </c>
-      <c r="D5" t="s">
-        <v>2</v>
-      </c>
       <c r="E5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2149</v>
       </c>
@@ -1064,19 +1151,22 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="D6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="G6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4532</v>
       </c>
@@ -1084,19 +1174,22 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="G7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4609</v>
       </c>
@@ -1104,19 +1197,22 @@
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="D8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="G8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4028</v>
       </c>
@@ -1124,19 +1220,22 @@
         <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="D9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="G9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>5766</v>
       </c>
@@ -1144,19 +1243,22 @@
         <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="D10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="G10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>5582</v>
       </c>
@@ -1164,19 +1266,22 @@
         <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="G11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>5714</v>
       </c>
@@ -1184,19 +1289,22 @@
         <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="D12" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="G12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>5437</v>
       </c>
@@ -1204,19 +1312,22 @@
         <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="D13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="G13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>4993</v>
       </c>
@@ -1224,19 +1335,22 @@
         <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="D14" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="G14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>5581</v>
       </c>
@@ -1244,19 +1358,22 @@
         <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="D15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="G15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>5909</v>
       </c>
@@ -1264,19 +1381,22 @@
         <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="D16" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="G16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>5107</v>
       </c>
@@ -1284,19 +1404,22 @@
         <v>20</v>
       </c>
       <c r="C17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" t="s">
         <v>8</v>
       </c>
-      <c r="D17" t="s">
-        <v>2</v>
-      </c>
       <c r="E17" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="G17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>6489</v>
       </c>
@@ -1304,19 +1427,22 @@
         <v>21</v>
       </c>
       <c r="C18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" t="s">
         <v>22</v>
       </c>
-      <c r="D18" t="s">
-        <v>2</v>
-      </c>
       <c r="E18" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F18" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="G18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>5125</v>
       </c>
@@ -1324,19 +1450,22 @@
         <v>23</v>
       </c>
       <c r="C19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" t="s">
         <v>22</v>
       </c>
-      <c r="D19" t="s">
-        <v>2</v>
-      </c>
       <c r="E19" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F19" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="G19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>5127</v>
       </c>
@@ -1344,19 +1473,22 @@
         <v>24</v>
       </c>
       <c r="C20" t="s">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="D20" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F20" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="G20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>6430</v>
       </c>
@@ -1364,19 +1496,22 @@
         <v>25</v>
       </c>
       <c r="C21" t="s">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="D21" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F21" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="G21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>5132</v>
       </c>
@@ -1384,19 +1519,23 @@
         <v>26</v>
       </c>
       <c r="C22" t="s">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="D22" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F22" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add abstract in tesis
</commit_message>
<xml_diff>
--- a/public/cursoTesis-2022/A2021-TRUJILLO.xlsx
+++ b/public/cursoTesis-2022/A2021-TRUJILLO.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\proyect-tesis-conta\public\cursoTesis-2022\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\sistema-tesis-upao-unt\public\cursoTesis-2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02803D57-7931-4089-8046-AC1CEFD1E1A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF63CC0B-0328-419B-991F-A46F38D587BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="A2021-TRUJILLO" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="55">
   <si>
     <t>NELSON OCTAVIO RUIZ CERDAN</t>
   </si>
@@ -31,9 +31,6 @@
     <t>Contabilidad y Finanzas</t>
   </si>
   <si>
-    <t>none</t>
-  </si>
-  <si>
     <t>DOMINGO ESTUARDO OLIVER LINARES</t>
   </si>
   <si>
@@ -103,9 +100,6 @@
     <t>MAURO CESAR ARMAS AGUILAR</t>
   </si>
   <si>
-    <t>null</t>
-  </si>
-  <si>
     <t>0000-0003-3388-4343</t>
   </si>
   <si>
@@ -170,6 +164,27 @@
   </si>
   <si>
     <t>0000-0003-3388-4364</t>
+  </si>
+  <si>
+    <t>orcid</t>
+  </si>
+  <si>
+    <t>categoria</t>
+  </si>
+  <si>
+    <t>carrera</t>
+  </si>
+  <si>
+    <t>direccion</t>
+  </si>
+  <si>
+    <t>correo</t>
+  </si>
+  <si>
+    <t>cod_docente</t>
+  </si>
+  <si>
+    <t>nombres</t>
   </si>
 </sst>
 </file>
@@ -1016,10 +1031,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1029,509 +1044,400 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>2641</v>
+      <c r="A1" t="s">
+        <v>53</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="E1" t="s">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="F1" t="s">
-        <v>3</v>
+        <v>51</v>
       </c>
       <c r="G1" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2841</v>
+        <v>2641</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
-      </c>
-      <c r="F2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>3387</v>
+        <v>2841</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D3" t="s">
         <v>1</v>
       </c>
       <c r="E3" t="s">
         <v>2</v>
-      </c>
-      <c r="F3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1179</v>
+        <v>3387</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D4" t="s">
         <v>1</v>
       </c>
       <c r="E4" t="s">
         <v>2</v>
-      </c>
-      <c r="F4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4113</v>
+        <v>1179</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E5" t="s">
         <v>2</v>
-      </c>
-      <c r="F5" t="s">
-        <v>3</v>
-      </c>
-      <c r="G5" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2149</v>
+        <v>4113</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E6" t="s">
         <v>2</v>
-      </c>
-      <c r="F6" t="s">
-        <v>3</v>
-      </c>
-      <c r="G6" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>4532</v>
+        <v>2149</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s">
         <v>1</v>
       </c>
       <c r="E7" t="s">
         <v>2</v>
-      </c>
-      <c r="F7" t="s">
-        <v>3</v>
-      </c>
-      <c r="G7" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>4609</v>
+        <v>4532</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D8" t="s">
         <v>1</v>
       </c>
       <c r="E8" t="s">
         <v>2</v>
-      </c>
-      <c r="F8" t="s">
-        <v>3</v>
-      </c>
-      <c r="G8" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>4028</v>
+        <v>4609</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D9" t="s">
         <v>1</v>
       </c>
       <c r="E9" t="s">
         <v>2</v>
-      </c>
-      <c r="F9" t="s">
-        <v>3</v>
-      </c>
-      <c r="G9" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>5766</v>
+        <v>4028</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s">
         <v>1</v>
       </c>
       <c r="E10" t="s">
         <v>2</v>
-      </c>
-      <c r="F10" t="s">
-        <v>3</v>
-      </c>
-      <c r="G10" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>5582</v>
+        <v>5766</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D11" t="s">
         <v>1</v>
       </c>
       <c r="E11" t="s">
         <v>2</v>
-      </c>
-      <c r="F11" t="s">
-        <v>3</v>
-      </c>
-      <c r="G11" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>5714</v>
+        <v>5582</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D12" t="s">
         <v>1</v>
       </c>
       <c r="E12" t="s">
         <v>2</v>
-      </c>
-      <c r="F12" t="s">
-        <v>3</v>
-      </c>
-      <c r="G12" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>5437</v>
+        <v>5714</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D13" t="s">
         <v>1</v>
       </c>
       <c r="E13" t="s">
         <v>2</v>
-      </c>
-      <c r="F13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G13" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>4993</v>
+        <v>5437</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D14" t="s">
         <v>1</v>
       </c>
       <c r="E14" t="s">
         <v>2</v>
-      </c>
-      <c r="F14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G14" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>5581</v>
+        <v>4993</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D15" t="s">
         <v>1</v>
       </c>
       <c r="E15" t="s">
         <v>2</v>
-      </c>
-      <c r="F15" t="s">
-        <v>3</v>
-      </c>
-      <c r="G15" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
+        <v>5581</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>5909</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>5107</v>
+      </c>
+      <c r="B18" t="s">
         <v>19</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>6489</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" t="s">
         <v>43</v>
       </c>
-      <c r="D16" t="s">
-        <v>1</v>
-      </c>
-      <c r="E16" t="s">
-        <v>2</v>
-      </c>
-      <c r="F16" t="s">
-        <v>3</v>
-      </c>
-      <c r="G16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>5107</v>
-      </c>
-      <c r="B17" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="D19" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>5125</v>
+      </c>
+      <c r="B20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" t="s">
         <v>44</v>
       </c>
-      <c r="D17" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" t="s">
-        <v>2</v>
-      </c>
-      <c r="F17" t="s">
-        <v>3</v>
-      </c>
-      <c r="G17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>6489</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="D20" t="s">
         <v>21</v>
       </c>
-      <c r="C18" t="s">
+      <c r="E20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>5127</v>
+      </c>
+      <c r="B21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" t="s">
         <v>45</v>
       </c>
-      <c r="D18" t="s">
-        <v>22</v>
-      </c>
-      <c r="E18" t="s">
-        <v>2</v>
-      </c>
-      <c r="F18" t="s">
-        <v>3</v>
-      </c>
-      <c r="G18" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>5125</v>
-      </c>
-      <c r="B19" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="D21" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>6430</v>
+      </c>
+      <c r="B22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" t="s">
         <v>46</v>
       </c>
-      <c r="D19" t="s">
-        <v>22</v>
-      </c>
-      <c r="E19" t="s">
-        <v>2</v>
-      </c>
-      <c r="F19" t="s">
-        <v>3</v>
-      </c>
-      <c r="G19" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>5127</v>
-      </c>
-      <c r="B20" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="D22" t="s">
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>5132</v>
+      </c>
+      <c r="B23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" t="s">
         <v>47</v>
       </c>
-      <c r="D20" t="s">
-        <v>1</v>
-      </c>
-      <c r="E20" t="s">
-        <v>2</v>
-      </c>
-      <c r="F20" t="s">
-        <v>3</v>
-      </c>
-      <c r="G20" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>6430</v>
-      </c>
-      <c r="B21" t="s">
-        <v>25</v>
-      </c>
-      <c r="C21" t="s">
-        <v>48</v>
-      </c>
-      <c r="D21" t="s">
-        <v>1</v>
-      </c>
-      <c r="E21" t="s">
-        <v>2</v>
-      </c>
-      <c r="F21" t="s">
-        <v>3</v>
-      </c>
-      <c r="G21" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>5132</v>
-      </c>
-      <c r="B22" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" t="s">
-        <v>49</v>
-      </c>
-      <c r="D22" t="s">
-        <v>1</v>
-      </c>
-      <c r="E22" t="s">
-        <v>2</v>
-      </c>
-      <c r="F22" t="s">
-        <v>3</v>
-      </c>
-      <c r="G22" t="s">
-        <v>27</v>
+      <c r="D23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Avance filtrar y buscar
</commit_message>
<xml_diff>
--- a/public/cursoTesis-2022/A2021-TRUJILLO.xlsx
+++ b/public/cursoTesis-2022/A2021-TRUJILLO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\sistema-tesis-upao-unt\public\cursoTesis-2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF63CC0B-0328-419B-991F-A46F38D587BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9F14F9E-FCFD-4E69-960F-9E503E2FE6EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="A2021-TRUJILLO" sheetId="1" r:id="rId1"/>
@@ -20,85 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="55">
-  <si>
-    <t>NELSON OCTAVIO RUIZ CERDAN</t>
-  </si>
-  <si>
-    <t>NOMBRADO</t>
-  </si>
-  <si>
-    <t>Contabilidad y Finanzas</t>
-  </si>
-  <si>
-    <t>DOMINGO ESTUARDO OLIVER LINARES</t>
-  </si>
-  <si>
-    <t>SANTIAGO NESTOR BOCANEGRA OSORIO</t>
-  </si>
-  <si>
-    <t>AUGUSTO RICARDO MORENO RODRIGUEZ</t>
-  </si>
-  <si>
-    <t>ROSA AMABLE SALCEDO DAVALOS</t>
-  </si>
-  <si>
-    <t>NOMBRADA</t>
-  </si>
-  <si>
-    <t>ANTONIO CHOLAN CALDERON</t>
-  </si>
-  <si>
-    <t>CRISTIAN AUSBERTO PARIMANGO REBAZA</t>
-  </si>
-  <si>
-    <t>WINSTON ROLANDO REAÑO PORTAL</t>
-  </si>
-  <si>
-    <t>JAIME GILBERTO MONTENEGRO RIOS</t>
-  </si>
-  <si>
-    <t>JUAN CARLOS MIRANDA ROBLES</t>
-  </si>
-  <si>
-    <t>YONI MATEO VALIENTE SALDAÑA</t>
-  </si>
-  <si>
-    <t>CESAR AUGUSTO HERRERA ASMAT</t>
-  </si>
-  <si>
-    <t>JORGE EDWIN MANTILLA SEVILLANO</t>
-  </si>
-  <si>
-    <t>JAVIER LEOPOLDO ULLOA SICCHA</t>
-  </si>
-  <si>
-    <t>RAFAEL EDUARDO PAREDES TEJADA</t>
-  </si>
-  <si>
-    <t>ALFREDO RUBEN SAAVEDRA RODRIGUEZ</t>
-  </si>
-  <si>
-    <t>ANA MARIA CUADRA MIDZUARAY</t>
-  </si>
-  <si>
-    <t>JUAN URQUIZO CUELLAR</t>
-  </si>
-  <si>
-    <t>CONTRATADO</t>
-  </si>
-  <si>
-    <t>ROLANDO DE LA CRUZ ASMAT</t>
-  </si>
-  <si>
-    <t>SARA ISABEL CABANILLAS ÑAÑO</t>
-  </si>
-  <si>
-    <t>RUBY MARILU LUJAN CHINININ</t>
-  </si>
-  <si>
-    <t>MAURO CESAR ARMAS AGUILAR</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>0000-0003-3388-4343</t>
   </si>
@@ -118,63 +40,12 @@
     <t>0000-0003-3388-4348</t>
   </si>
   <si>
-    <t>0000-0003-3388-4349</t>
-  </si>
-  <si>
-    <t>0000-0003-3388-4350</t>
-  </si>
-  <si>
-    <t>0000-0003-3388-4351</t>
-  </si>
-  <si>
-    <t>0000-0003-3388-4352</t>
-  </si>
-  <si>
-    <t>0000-0003-3388-4353</t>
-  </si>
-  <si>
-    <t>0000-0003-3388-4354</t>
-  </si>
-  <si>
-    <t>0000-0003-3388-4355</t>
-  </si>
-  <si>
-    <t>0000-0003-3388-4356</t>
-  </si>
-  <si>
-    <t>0000-0003-3388-4357</t>
-  </si>
-  <si>
-    <t>0000-0003-3388-4358</t>
-  </si>
-  <si>
-    <t>0000-0003-3388-4359</t>
-  </si>
-  <si>
-    <t>0000-0003-3388-4360</t>
-  </si>
-  <si>
-    <t>0000-0003-3388-4361</t>
-  </si>
-  <si>
-    <t>0000-0003-3388-4362</t>
-  </si>
-  <si>
-    <t>0000-0003-3388-4363</t>
-  </si>
-  <si>
-    <t>0000-0003-3388-4364</t>
-  </si>
-  <si>
     <t>orcid</t>
   </si>
   <si>
     <t>categoria</t>
   </si>
   <si>
-    <t>carrera</t>
-  </si>
-  <si>
     <t>direccion</t>
   </si>
   <si>
@@ -185,13 +56,55 @@
   </si>
   <si>
     <t>nombres</t>
+  </si>
+  <si>
+    <t>grado_academico</t>
+  </si>
+  <si>
+    <t>apellidos</t>
+  </si>
+  <si>
+    <t>RUIZ CERDAN</t>
+  </si>
+  <si>
+    <t>OLIVER LINARES</t>
+  </si>
+  <si>
+    <t>BOCANEGRA OSORIO</t>
+  </si>
+  <si>
+    <t>MORENO RODRIGUEZ</t>
+  </si>
+  <si>
+    <t>SALCEDO DAVALOS</t>
+  </si>
+  <si>
+    <t>CHOLAN CALDERON</t>
+  </si>
+  <si>
+    <t>ANTONIO</t>
+  </si>
+  <si>
+    <t>ROSA AMABLE</t>
+  </si>
+  <si>
+    <t>AUGUSTO RICARDO</t>
+  </si>
+  <si>
+    <t>SANTIAGO NESTOR</t>
+  </si>
+  <si>
+    <t>DOMINGO ESTUARDO</t>
+  </si>
+  <si>
+    <t>NELSON OCTAVIO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -328,6 +241,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -674,8 +595,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1031,417 +953,131 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="39.140625" customWidth="1"/>
-    <col min="5" max="5" width="31.140625" customWidth="1"/>
+    <col min="2" max="4" width="39.140625" customWidth="1"/>
+    <col min="6" max="6" width="31.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>54</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>49</v>
+        <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="F1" t="s">
-        <v>51</v>
+        <v>7</v>
       </c>
       <c r="G1" t="s">
-        <v>52</v>
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2641</v>
       </c>
       <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2841</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3387</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1179</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4113</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2149</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>31</v>
+        <v>20</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>4532</v>
-      </c>
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>4609</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" t="s">
-        <v>1</v>
-      </c>
-      <c r="E9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>4028</v>
-      </c>
-      <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" t="s">
-        <v>1</v>
-      </c>
-      <c r="E10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>5766</v>
-      </c>
-      <c r="B11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" t="s">
-        <v>1</v>
-      </c>
-      <c r="E11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>5582</v>
-      </c>
-      <c r="B12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" t="s">
-        <v>1</v>
-      </c>
-      <c r="E12" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>5714</v>
-      </c>
-      <c r="B13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" t="s">
-        <v>1</v>
-      </c>
-      <c r="E13" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>5437</v>
-      </c>
-      <c r="B14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" t="s">
-        <v>1</v>
-      </c>
-      <c r="E14" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>4993</v>
-      </c>
-      <c r="B15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" t="s">
-        <v>1</v>
-      </c>
-      <c r="E15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>5581</v>
-      </c>
-      <c r="B16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" t="s">
-        <v>40</v>
-      </c>
-      <c r="D16" t="s">
-        <v>1</v>
-      </c>
-      <c r="E16" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>5909</v>
-      </c>
-      <c r="B17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" t="s">
-        <v>1</v>
-      </c>
-      <c r="E17" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>5107</v>
-      </c>
-      <c r="B18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>6489</v>
-      </c>
-      <c r="B19" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" t="s">
-        <v>43</v>
-      </c>
-      <c r="D19" t="s">
-        <v>21</v>
-      </c>
-      <c r="E19" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>5125</v>
-      </c>
-      <c r="B20" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" t="s">
-        <v>44</v>
-      </c>
-      <c r="D20" t="s">
-        <v>21</v>
-      </c>
-      <c r="E20" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>5127</v>
-      </c>
-      <c r="B21" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" t="s">
-        <v>45</v>
-      </c>
-      <c r="D21" t="s">
-        <v>1</v>
-      </c>
-      <c r="E21" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>6430</v>
-      </c>
-      <c r="B22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" t="s">
-        <v>1</v>
-      </c>
-      <c r="E22" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>5132</v>
-      </c>
-      <c r="B23" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" t="s">
-        <v>47</v>
-      </c>
-      <c r="D23" t="s">
-        <v>1</v>
-      </c>
-      <c r="E23" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>